<commit_message>
Update data for lab 7
</commit_message>
<xml_diff>
--- a/Data_Sets/Lab_7-ghg-concentrations.xlsx
+++ b/Data_Sets/Lab_7-ghg-concentrations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beebee/Documents/GitHub/Intro-Stats-Excel-Lab-Manual/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/beebee/Documents/GitHub/Intro-Stats-Excel-Lab-Manual/Data_Sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{1C279120-39AC-3142-96E8-45614B3D3D52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B0A835-C197-4549-84E6-1828BE4BE8AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ghg-concentrations_fig-1" sheetId="1" r:id="rId1"/>
@@ -58,13 +58,13 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Global Atmospheric Concentrations of Carbon Dioxide Over Time</t>
+    <t>Global Atmospheric Concentrations of Carbon Dioxide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -898,12 +898,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>